<commit_message>
Updated sample file and changed the column name to match the file
</commit_message>
<xml_diff>
--- a/test/sample_tablebase.xlsx
+++ b/test/sample_tablebase.xlsx
@@ -3,7 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet2" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Matrix" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Workers" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Payor Matrix Weighted Invoice Count Scoring Table</t>
   </si>
@@ -161,6 +162,42 @@
   </si>
   <si>
     <t>WORKERS COMPENSATION</t>
+  </si>
+  <si>
+    <t>Agent</t>
+  </si>
+  <si>
+    <t>Silva, Flavio</t>
+  </si>
+  <si>
+    <t>Gomez, Manuel</t>
+  </si>
+  <si>
+    <t>Bertone, Ignacio</t>
+  </si>
+  <si>
+    <t>Pereira,Eugenia</t>
+  </si>
+  <si>
+    <t>Taborda, Lucia</t>
+  </si>
+  <si>
+    <t>Gallinar,Romina</t>
+  </si>
+  <si>
+    <t>Oliver, Matilde</t>
+  </si>
+  <si>
+    <t>Alvez, Eugenia</t>
+  </si>
+  <si>
+    <t>Florin, Steban</t>
+  </si>
+  <si>
+    <t>Rodriguez, Ginni</t>
+  </si>
+  <si>
+    <t>Gill, Angela</t>
   </si>
 </sst>
 </file>
@@ -286,6 +323,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1561,4 +1602,82 @@
   </conditionalFormatting>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="13.38"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>